<commit_message>
fix: SonarQube fixes and implementation of constants
</commit_message>
<xml_diff>
--- a/src/Services/test.xlsx
+++ b/src/Services/test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renzi\Documents\FING\PIS\repp_backend\src\Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10AA738-25F3-4359-BA22-FD0BEFE45BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81351AF1-327E-4D12-8870-1FCCE0B3D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{A4031272-87DC-43E9-BA95-7EFE4AF5910A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A4031272-87DC-43E9-BA95-7EFE4AF5910A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hombres&lt;1" sheetId="1" r:id="rId1"/>
     <sheet name="Hombres" sheetId="2" r:id="rId2"/>
     <sheet name="Mujeres&lt;1" sheetId="4" r:id="rId3"/>
+    <sheet name="Mujeres" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>*En caso de no tener el peso de la persona, se puede ingresar la talla en su defecto</t>
   </si>
@@ -647,13 +648,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="10"/>
-    <col min="2" max="2" width="12.1796875" style="4"/>
+    <col min="1" max="1" width="12.140625" style="10"/>
+    <col min="2" max="2" width="12.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
@@ -665,7 +666,7 @@
       </c>
       <c r="P1" s="14"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>9</v>
       </c>
@@ -675,7 +676,7 @@
       <c r="O2" s="15"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>11</v>
       </c>
@@ -685,67 +686,67 @@
       <c r="O3" s="15"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O4" s="17"/>
       <c r="P4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
@@ -763,17 +764,17 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:N9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="5"/>
-    <col min="3" max="3" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -784,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>14</v>
       </c>
@@ -795,7 +796,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>13</v>
       </c>
@@ -806,7 +807,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K4" s="19" t="s">
         <v>0</v>
       </c>
@@ -814,31 +815,31 @@
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
@@ -856,17 +857,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F03E005-0A22-4DA5-A050-9B514C55239F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="12.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -874,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>7</v>
       </c>
@@ -887,22 +888,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7D79B8-0D84-4480-A012-8644393D2706}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D5A9C43658ED8F47B0DE71BE080C72CD" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="3a0a1906cd942b854ebba9dcb7c59828">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0429e6f6-3210-4cd6-acdf-ec68178a7607" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47a910d12d0e99a366a53a773091406" ns2:_="">
     <xsd:import namespace="0429e6f6-3210-4cd6-acdf-ec68178a7607"/>
@@ -1086,24 +1118,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96791853-1F35-43CC-95E3-7FA1F9E37EC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51903091-7D99-4F5E-8DEE-30AC40088B6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F379961-77C4-4F40-B977-E17376CE4E90}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1119,4 +1149,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51903091-7D99-4F5E-8DEE-30AC40088B6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96791853-1F35-43CC-95E3-7FA1F9E37EC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: sheetParser now returns an ageGroup array
</commit_message>
<xml_diff>
--- a/src/Services/test.xlsx
+++ b/src/Services/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renzi\Documents\FING\PIS\repp_backend\src\Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81351AF1-327E-4D12-8870-1FCCE0B3D87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A28E6BB-4C09-4883-8B53-5AD177DCB1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{A4031272-87DC-43E9-BA95-7EFE4AF5910A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{A4031272-87DC-43E9-BA95-7EFE4AF5910A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hombres&lt;1" sheetId="1" r:id="rId1"/>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7D79B8-0D84-4480-A012-8644393D2706}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +927,30 @@
       </c>
       <c r="C3" s="4">
         <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>